<commit_message>
[WIP] Allow for data source independence (json, excel, testng parameter)
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheetData/changeLager/Example.xlsx
+++ b/src/test/resources/spreadsheetData/changeLager/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EclipseWorkspace\New\SeleniumFramework\src\test\resources\spreadsheetData\changeLager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3F5D1F98-EF33-42B2-B036-1CA237804D90}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{391D860B-7C02-4196-A7B2-AFB3AB1EA201}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
   </bookViews>
@@ -701,7 +701,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2D1F1-7BA5-4534-88B6-D969E332B0E1}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -833,7 +835,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>

</xml_diff>